<commit_message>
falta descarga de pdf
</commit_message>
<xml_diff>
--- a/usuarios.xlsx
+++ b/usuarios.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenzo Orozco\Desktop\embeding\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770133CC-874F-4ED4-9476-E5F010B3A1BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="2028" yWindow="696" windowWidth="18660" windowHeight="9984" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -34,19 +28,19 @@
     <t>Mario</t>
   </si>
   <si>
+    <t>Bronce</t>
+  </si>
+  <si>
     <t>testuser</t>
   </si>
   <si>
+    <t>testpassword</t>
+  </si>
+  <si>
+    <t>Plata</t>
+  </si>
+  <si>
     <t>peach</t>
-  </si>
-  <si>
-    <t>testpassword</t>
-  </si>
-  <si>
-    <t>Bronce</t>
-  </si>
-  <si>
-    <t>Plata</t>
   </si>
   <si>
     <t>Oro</t>
@@ -55,8 +49,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,10 +62,15 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -81,7 +81,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -91,54 +91,76 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+  <cellXfs count="8">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -171,79 +193,79 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -264,54 +286,53 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
+                <a:tint val="15000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
+                <a:tint val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
+              <a:shade val="9500"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -321,7 +342,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -330,7 +351,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -339,7 +360,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -347,10 +368,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -379,7 +400,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
+                <a:tint val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -392,13 +413,12 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -416,56 +436,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="4">
         <v>123</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
+      <c r="B4" s="4">
         <v>123</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se crea un esqueleto del dashboard, es dinamico
</commit_message>
<xml_diff>
--- a/usuarios.xlsx
+++ b/usuarios.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenzo Orozco\Documents\GitHub\ProyectoEva_embeding\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5558FBE-DB04-48DA-BC1A-84B890492625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>nombre_usuario</t>
   </si>
@@ -31,12 +37,6 @@
     <t>Bronce</t>
   </si>
   <si>
-    <t>testuser</t>
-  </si>
-  <si>
-    <t>testpassword</t>
-  </si>
-  <si>
     <t>Plata</t>
   </si>
   <si>
@@ -44,13 +44,27 @@
   </si>
   <si>
     <t>Oro</t>
+  </si>
+  <si>
+    <t>Batería</t>
+  </si>
+  <si>
+    <t>Mensajes</t>
+  </si>
+  <si>
+    <t>Viajes</t>
+  </si>
+  <si>
+    <t>luigi</t>
+  </si>
+  <si>
+    <t>Geocercas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -115,38 +129,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -157,10 +165,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -198,71 +206,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -290,7 +298,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -313,11 +321,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -326,13 +334,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -342,7 +350,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -351,7 +359,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -360,7 +368,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -368,10 +376,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -436,22 +444,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row r="1" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -461,38 +471,86 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>123</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4">
+        <v>123</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B4" s="3">
+        <v>123</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="4">
-        <v>123</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Te muestra mensajes si la columna mensajes tienen un 1 en el excel, tambien la descarga de PDF fue mejorada
</commit_message>
<xml_diff>
--- a/usuarios.xlsx
+++ b/usuarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenzo Orozco\Documents\GitHub\ProyectoEva_embeding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5558FBE-DB04-48DA-BC1A-84B890492625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{751E7811-7234-4705-A1A5-5FD6A26FA040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31500" yWindow="2955" windowWidth="17310" windowHeight="8895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -451,7 +451,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Ya está el embeding de EVA, cambio de logo en el login
</commit_message>
<xml_diff>
--- a/usuarios.xlsx
+++ b/usuarios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenzo Orozco\Documents\GitHub\ProyectoEva_embeding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{751E7811-7234-4705-A1A5-5FD6A26FA040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715496D6-2B68-4184-9CEC-3C0BDE5E0A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31500" yWindow="2955" windowWidth="17310" windowHeight="8895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,9 +49,6 @@
     <t>Batería</t>
   </si>
   <si>
-    <t>Mensajes</t>
-  </si>
-  <si>
     <t>Viajes</t>
   </si>
   <si>
@@ -59,6 +56,9 @@
   </si>
   <si>
     <t>Geocercas</t>
+  </si>
+  <si>
+    <t>Consulta de sensor</t>
   </si>
 </sst>
 </file>
@@ -451,7 +451,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -475,13 +475,13 @@
         <v>8</v>
       </c>
       <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -509,7 +509,7 @@
     </row>
     <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="4">
         <v>123</v>

</xml_diff>

<commit_message>
esta todo lo de notificaciones pero la grafica de geocercas se encima en mensaje
</commit_message>
<xml_diff>
--- a/usuarios.xlsx
+++ b/usuarios.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenzo Orozco\Documents\GitHub\ProyectoEva_embeding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715496D6-2B68-4184-9CEC-3C0BDE5E0A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA41974-FEE3-434A-B094-4B4C9E3AF7A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31500" yWindow="2955" windowWidth="17310" windowHeight="8895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31500" yWindow="2955" windowWidth="17310" windowHeight="8895" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sensores" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>nombre_usuario</t>
   </si>
@@ -59,6 +60,12 @@
   </si>
   <si>
     <t>Consulta de sensor</t>
+  </si>
+  <si>
+    <t>ThinkPower  TL904D</t>
+  </si>
+  <si>
+    <t>AOVX GM100</t>
   </si>
 </sst>
 </file>
@@ -450,8 +457,8 @@
   </sheetPr>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -556,4 +563,63 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B122E974-7193-4DC1-915D-6244D8FCB5FC}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
se desorganiza pero si es variable el dashboard
</commit_message>
<xml_diff>
--- a/usuarios.xlsx
+++ b/usuarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenzo Orozco\Documents\GitHub\ProyectoEva_embeding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA41974-FEE3-434A-B094-4B4C9E3AF7A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5256A51E-A26C-4EB2-A227-7489AA0FBC00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31500" yWindow="2955" windowWidth="17310" windowHeight="8895" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -457,8 +457,8 @@
   </sheetPr>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -569,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B122E974-7193-4DC1-915D-6244D8FCB5FC}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
funciona ya la fecha y login, ando con la gráfica de bateria
</commit_message>
<xml_diff>
--- a/usuarios.xlsx
+++ b/usuarios.xlsx
@@ -533,7 +533,11 @@
       <c r="G3" t="n">
         <v>0</v>
       </c>
-      <c r="H3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>af2d19bdad5bcc3708bcb2b9f32ccaf49E6BF287EE7E19ED8F9ADA2F466A0CBD4C488B69</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -563,7 +567,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>41454459d97f26fb5c2f8815b477a754E0E84B079762B1026659BC5014D359511EA07499</t>
+          <t>41454459d97f26fb5c2f8815b477a754FBAA0E440484A2E6480F313AAE783C9595E20036</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
ya se muestran las 2 graficas, no se pueden ver valores individuales ni descarga en excel pero funcionan bien
</commit_message>
<xml_diff>
--- a/usuarios.xlsx
+++ b/usuarios.xlsx
@@ -1,37 +1,96 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t>nombre_usuario</t>
+  </si>
+  <si>
+    <t>contrasena</t>
+  </si>
+  <si>
+    <t>tipo_plan</t>
+  </si>
+  <si>
+    <t>Batería</t>
+  </si>
+  <si>
+    <t>Consulta de sensor</t>
+  </si>
+  <si>
+    <t>Viajes</t>
+  </si>
+  <si>
+    <t>Geocercas</t>
+  </si>
+  <si>
+    <t>wialon_token</t>
+  </si>
+  <si>
+    <t>Mario</t>
+  </si>
+  <si>
+    <t>luigi</t>
+  </si>
+  <si>
+    <t>peach</t>
+  </si>
+  <si>
+    <t>Bronce</t>
+  </si>
+  <si>
+    <t>Plata</t>
+  </si>
+  <si>
+    <t>Oro</t>
+  </si>
+  <si>
+    <t>41454459d97f26fb5c2f8815b477a754A8CE3BB3A1C0FDEB0E2ED4543051B232FF634D2E</t>
+  </si>
+  <si>
+    <t>af2d19bdad5bcc3708bcb2b9f32ccaf49E6BF287EE7E19ED8F9ADA2F466A0CBD4C488B69</t>
+  </si>
+  <si>
+    <t>41454459d97f26fb5c2f8815b477a75483A25333FC2FAC9A19D5589AA5C6F16294533942</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +105,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -420,158 +421,118 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>nombre_usuario</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>contrasena</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>tipo_plan</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Batería</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Consulta de sensor</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Viajes</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Geocercas</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>wialon_token</t>
-        </is>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Mario</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
         <v>123</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Bronce</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>41454459d97f26fb5c2f8815b477a754A8CE3BB3A1C0FDEB0E2ED4543051B232FF634D2E</t>
-        </is>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>luigi</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
         <v>123</v>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Plata</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>af2d19bdad5bcc3708bcb2b9f32ccaf49E6BF287EE7E19ED8F9ADA2F466A0CBD4C488B69</t>
-        </is>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>peach</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
         <v>123</v>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Oro</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>1</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4">
         <v>1</v>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>41454459d97f26fb5c2f8815b477a754C6EE63274CD297843A09C86FA6E08CF482AF0BBA</t>
-        </is>
+      <c r="H4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Nuevo dash con envio de datos al back en conexion pero hay un desastre en que reporte ejecuta cada uno
</commit_message>
<xml_diff>
--- a/usuarios.xlsx
+++ b/usuarios.xlsx
@@ -1,27 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PcR\Documents\GitHub\ProyectoEva_embeding\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B3835E-E3EB-4C84-9B02-37989A88F971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3735" yWindow="1500" windowWidth="21375" windowHeight="13980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sensores" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>nombre_usuario</t>
   </si>
@@ -44,6 +37,12 @@
     <t>Geocercas</t>
   </si>
   <si>
+    <t>Conexion</t>
+  </si>
+  <si>
+    <t>wialon_token</t>
+  </si>
+  <si>
     <t>Mario</t>
   </si>
   <si>
@@ -62,20 +61,14 @@
     <t>Oro</t>
   </si>
   <si>
-    <t>Thinkpower</t>
-  </si>
-  <si>
-    <t>AOVX GL100</t>
-  </si>
-  <si>
-    <t>Conexion</t>
+    <t>41454459d97f26fb5c2f8815b477a754976B44F8079D25BD1F3FB3F34FE39D2DC0BB7AD3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,21 +131,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -190,7 +175,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -224,7 +209,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -259,10 +243,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -435,16 +418,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -467,70 +448,73 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>123</v>
       </c>
       <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
         <v>10</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
       </c>
       <c r="B3">
         <v>123</v>
       </c>
       <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
         <v>11</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
       </c>
       <c r="B4">
         <v>123</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -547,64 +531,8 @@
       <c r="H4">
         <v>1</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B70D8BC-86B2-4299-9B6F-E47F53C14827}">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
+      <c r="I4" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>